<commit_message>
Update Sam Filter project for deployment
</commit_message>
<xml_diff>
--- a/data/my_solicitations.xlsx
+++ b/data/my_solicitations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,32 +518,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>M6786125Q0060</t>
+          <t>1240LT25Q0061</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ski Supplies</t>
+          <t>Kyle Canyon Bunkhouse HVAC Replacement</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>See Solicitation/Salient Characteristics.</t>
+          <t>Project Name: Kyle Canyon Bunkhouse HVAC Replacement Project Description: This work consists of replacement of an HVAC system at the Kyle Canyon Bunkhouse in the Spring Mountains National Recreation area in the Humboldt-Toiyabe National Forest. The project including removal and disposal of existing furnace, cooling coil and condensing units, in addition to the installation of a new HVAC system with a high altitude conversion kit and liquid propane conversion kit. Project Location: Spring Mountains Recreation Area Bunkhouse (36°16'17.67"N 115°33'46.84"W) Clark County, Nevada Pre-Proposal Site Visit Scheduled? No, see Section L. If interested in a site visit, contact the COR to request. (Dakota.Krist@usda.gov) Schedule Note: The period of performance dates are intended as a timeframe for when the project should be completed (i.e. between October 2025 and March 2026). Once work begins, the awardee will have 30 calendar days to complete the work (Contract time). Submit proposals to Westley.Bisson@usda.gov. Do not mail proposals.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sep 11, 2025 11:00 AM CDT</t>
+          <t>Oct 10, 2025 05:00 PM MDT</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 12, 2025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 12, 2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Dayton J. Greenwalt | Jordyn Edwards</t>
+          <t>Westley Bisson</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -561,20 +561,36 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Sporting and Athletic Goods Manufacturing</t>
+          <t>Plumbing, Heating, and Air-Conditioning Contractors</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>ATHLETIC AND SPORTING EQUIPMENT</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr"/>
+          <t>MAINT/REPAIR/REBUILD OF EQUIPMENT- REFRIGERATION, AIR CONDITIONING, AND AIR CIRCULATING EQUIPMENT</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr">
         <is>
           <t>Total Small Business Set-Aside (FAR 19.5)</t>
@@ -584,42 +600,42 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>W81K0425QA032</t>
+          <t>30471PR250000008</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pressure Monitoring Unit</t>
+          <t>Repair and Install HVAC at USCG STA Morro Bay</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>This is a Combined Synopsis/Solicitation. Please refer to the attached W81K0425QA032.</t>
+          <t>See the attached document for information. Direct all questions to the contracting officer and contract specialist (shawn.t.jenkins@uscg.mil and jesus.c.yutig.civ@uscg.mil). All offers must be emailed to the contracting officer and contract specialist by the closing date and time.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sep 18, 2025 01:00 PM EDT</t>
+          <t>Sep 19, 2025 03:00 PM EDT</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 13, 2025</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 13, 2025</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Combined Synopsis/Solicitation</t>
+          <t>Solicitation</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Justin Balster</t>
+          <t>Shawn Jenkins | Jesse Yutig</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -627,20 +643,36 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Electromedical and Electrotherapeutic Apparatus Manufacturing</t>
+          <t>Plumbing, Heating, and Air-Conditioning Contractors</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>MED &amp; SURGICAL INSTRUMENTS,EQ &amp; SUP</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr"/>
+          <t>MAINTENANCE OF OTHER ADMINISTRATIVE FACILITIES AND SERVICE BUILDINGS</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr">
         <is>
           <t>Total Small Business Set-Aside (FAR 19.5)</t>
@@ -650,42 +682,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>140R4025Q0094</t>
+          <t>30890PR250000020</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Glen Canyon Molded Case Circuit Breaker Replacemen</t>
+          <t>Replace HVAC at USCG STA Rio Vista</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>B1G board 125VDC Molded Case Circuit Breaker</t>
+          <t>See the attached document for information. Direct all questions to the contracting officer and contract specialist (shawn.t.jenkins@uscg.mil and jesus.c.yutig.civ@uscg.mil). All offers must be emailed to the contracting officer and contract specialist by the closing date and time.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Sep 16, 2025 05:00 PM MDT</t>
+          <t>Sep 19, 2025 03:00 PM EDT</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 13, 2025</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 13, 2025</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Combined Synopsis/Solicitation</t>
+          <t>Solicitation</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Romine, Michelle</t>
+          <t>Shawn Jenkins</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -693,20 +725,36 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Switchgear and Switchboard Apparatus Manufacturing</t>
+          <t>Plumbing, Heating, and Air-Conditioning Contractors</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>CIRCUIT BREAKERS</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr"/>
+          <t>MAINTENANCE OF OTHER ADMINISTRATIVE FACILITIES AND SERVICE BUILDINGS</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr">
         <is>
           <t>Total Small Business Set-Aside (FAR 19.5)</t>
@@ -716,42 +764,42 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>127EAV25Q0061</t>
+          <t>70Z028-25-Q-ASMHVACMAINTENANCE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pacific Valley Generator Replacement</t>
+          <t>USCG Air Station Miami FY26 HVAC Maintenance</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>The Los Padres National Forest has a need for the supply and installation of one 25kW propane generator at Pacific Valley Fire Station. This 25kW standby generator will charge the back-up battery system for primary solar-powered site. The generator shall be a Cummins Series RS25 or the equivalent by industry standards. Questions may be submitted to Christopher Malley, CS, at christopher.malley@usda.gov NLT 9/17/25. Quote packages may be submitted electronically via e-mail to the Contract Specialist at Christopher.malley@usda.gov</t>
+          <t>This combined synopsis/solicitation for services is prepared in accordance with the format in subpart 12.6 of the Federal Acquisition Regulation (FAR) as supplemented with additional information included in this notice. This synopsis/solicitation is being advertised as Small Business Set-Aside only. This announcement constitutes the only solicitation; no separate written solicitation will be issued. The solicitation number is 70Z028-25-Q-ASMHVACMAINTENANCE Applicable North American Industry Classification Standard (NAICS) codes are: NAICS 238220 - Plumbing, Heating, and Air-Conditioning Contractors Size standard: $19.0 million This requirement is for a firm fixed price services contract. The contract will be awarded using simplified acquisition procedures in accordance with FAR part 12 and FAR Part 13 The Government will award a contract resulting from this solicitation to the responsible offeror whose offer conforming to the solicitation will be most advantageous to the Government, LOWEST PRICE, TECHNICALLY ACCEPTABLE (LPTA). When submitting your proposals, request a price breakdown of the following: a. The cost of monthly HVAC maintenance as outlined in the Statement of Work (SOW), divided into 12 equal monthly payments. b. The annual cost for the Base Year plus 03 Option Years, with pricing for each option year broken down into 12 equal monthly payments. Prospective contractors must also provide, along with your proposal, past performance documents which will be used to determine expertise to perform the work requested. Contract will be awarded to the vendor who can perform the work outlined in the provided PWS in the time frame needed by unit. Award date: 05 business days after close of solicitation, 17 September 2025 Quotes are to be received no later than close of business 11 a.m. on 17 September 2025. Quotes can be email to: Arlett.Maj@uscg.mil Telephone requests of quotes will not be accepted, a formal notice of changes (if applicable) will be issued in Sam.Gov Wage determinations: Service Contract Act WD #: 2015-4543 County: Dade Rev: 32. Date: 07/08/2025 SCOPE OF WORK: To provide Air Station Miami HVAC Maintenane services required on a regular basis for the Air-Cooled Chiller on the NW side of the hangar building, the Water-Cooled Chiller adjacent to the galley building, and the Cooling tower adjacent to the Water-Cooled Chiller at Coast Guard Air Station Miami, Opa Locka, Florida, as defined in the Scope of Work. Location: USCG Air Station Miami 14750 NW 44th Ct Opa Locka, FL 33054 Period of Performance: Performance of work is expected to commence October 1, 2025 Period of Performance: October 1, 2025 – September 30, 2026 52.217-9 Option to Extend the Term of the Contract The Government may extend the term of this contract by written notice to the Contractor provided that the Government gives the Contractor a preliminary written notice of its intent to extend at least __60___ days before the contract expires. The preliminary notice does not commit the Government to an extension. (b) If the Government exercises this option, the extended contract shall be considered to include this option clause. USCG ASM HVAC MAINTENANCE (c) The total duration of this contract, including the exercising of any options under this clause, shall not exceed 48 months. Site visit: It is recommended but not mandatory that a site visit is performed at the Unit to verify the requirements within the PWS and speak with the unit POC for this service. Vendors shall contact: POC: LT Thomas Jones Email: Thomas.M.Jones@uscg.mil Phone: (443) 262-2838 Q&amp;A’s: Questions concerning the work requested must be sent to Arlett.Maj@uscg.mil by COB September 9, 2025. These Q&amp;A’s will be answered and posted to this solicitation as an amendment to solicitation prior to close. 52.212-1 -- Instructions to Offerors -- Commercial Items. (DEVIATION 2018-O0018) Instructions to Offerors -- Commercial Items (June 2020) 52.212-3 Offeror Representations and Certifications -- Commercial Items (June 2020) Work hours: Monday through Friday, 0800 – 1500 (8 am – 3 pm) See attached applicable FAR Clauses by reference. Offerors may obtain a full text version of these clauses electronically at: www.arnet.gov/far The following Homeland Security Acquisition Regulations (HSAR) are incorporated as addenda to this solicitation: HSAR 3052.209-70 Prohibition on Contracts with Corporate Expatriates (Jun 2006); Contracting Officers Technical Representative (Dec 2003) (COTR) HSAR 3052.237-72. Copies of HSAR clauses may be obtained electronically at http://www.dhs.gov. Request Company’s tax ID information and UEI number. Vendors providing an offer must be registered in SAM (System for Award Management) prior to close of this solicitation. https://www.sam.gov/portal/public/SAM/. The vendors SAM registration must be in an “ACTIVE” status prior to award. Vendors must ensure that the above listed NAICS codes are listed on their SAM registration to perform this type of service. The Government reserves the right to cancel this solicitation at any time.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sep 25, 2025 01:00 PM PDT</t>
+          <t>Sep 17, 2025 11:00 AM EDT</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 4, 2025</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sep 11, 2025</t>
+          <t>Sep 4, 2025</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Solicitation</t>
+          <t>Combined Synopsis/Solicitation</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Christopher Malley</t>
+          <t>SK1 Arlett Maj | SK1 Alera Nash</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -759,169 +807,37 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Electrical Contractors and Other Wiring Installation Contractors</t>
+          <t>Plumbing, Heating, and Air-Conditioning Contractors</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>GENERATORS &amp; GENERATOR SETS ELECT</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr"/>
+          <t>MAINT/REPAIR/REBUILD OF EQUIPMENT- REFRIGERATION, AIR CONDITIONING, AND AIR CIRCULATING EQUIPMENT</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr">
-        <is>
-          <t>Total Small Business Set-Aside (FAR 19.5)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FA461325R0010</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Demolition of Ammo Buildings</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Mo/Year: September 2025 Contracting Office Zip Code: 82005-2860 Product Service Code: P400 Contracting Office Address: 90th Contracting Squadron, 7505 Barnes Loop, Bldg 208, F. E. Warren AFB, W.Y. Subject: Combined Synopsis/Solicitation; Demolition of Buildings 2242 and 2243 Solicitation Number: FA461325R0010 Closing Response Date: 24 September 2025; 10:00 a.m. MDT Contact POC: TSgt Chad Evans, 307-773-6648 chad.evans.19@us.af.mil or Mr. Arthur Makekau, 307-773-6829 arthur.makekau@us.af.mil. Line Items (CLINs): See Attachment 1 and Attachment 5 for full description, details, delivery &amp; acceptance and base plus bid option information. Description: This is a combined synopsis/solicitation for commercial products or services prepared in accordance with the format in subpart 12.6, as supplemented with additional information included in this notice. This announcement will include an attached solicitation in which quotes are being requested. This solicitation will be posted to Contract Opportunities found on the SAM.Gov website as a 100% Small Business Set Aside. The 90th Contracting Squadron is issuing this combined synopsis/solicitation, FA461325R0010, as a Request for Proposal (RFP). The solicitation document and incorporated provisions and clauses are those in effect through the Federal Acquisition Circular (FAC) 2025-05 effective 08/07/2025, Defense Federal Acquisition Regulation Change 01/17/2025 effective 01/17/2025 and Department of the Air Force Federal Acquisition Regulation Supplement DAFFARS Change 10/16/2024 effective 10/16/2024. As a 100% small business set-aside, this RFP utilizes FAR Part 12, Acquisition of Commercial Products and Services, &amp; FAR Part 13.5, Simplified Acquisition Procedures. The North American Industrial Classification System (NAICS) code is 238910, with a small business standard of $19M. The Government intends to award a contract to a small business to provide demolition services for two to five WWII era ammo storage buildings located on F. E. Warren AFB, WY. The description and list of the CLIN line-item number(s), quantities, units of measure for the base and bid options are specified in the solicitation. *** Site Visit on 18 September 2025 10:00 a.m. MDT*** ***Questions due NLT 19 September 2025; 2:00 p.m. MDT*** ***Proposals due NLT 24 September 2025; 10:00 a.m. MDT*** NOTES: Refer to each attachment(s) for full instructions and details. Quotes must be signed, dated and submitted by the date indicated above. In addition to the quote, submit Vendor’s CAGE code, DUNS number, Tax Identification Number, Prompt Payment Terms, Delivery Time, Date offer expires, warranty, Line-item unit price, and Total costs (base bid plus (2) bid options). Proposals shall be emailed to TSgt Chad Evans, 307-773-6648 chad.evans.19@us.af.mil and Mr. Arthur Makekau, 307-773-6829 arthur.makekau@us.af.mil. ATTACHMENTS: Attachment 1: PWS 21 Aug 2025 Attachment 2: Asbestos Inspection Report Attachment 3: WD 2015-5405 Rev 26 8JUL25 Attachment 4: Environmental Specifications Feb2024 Attachment 5: Solicitation - FA461325R0010</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Sep 24, 2025 10:00 AM MDT</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Sep 11, 2025</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Sep 11, 2025</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Combined Synopsis/Solicitation</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Chad Evans | Arthur Makekau</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Site Preparation Contractors</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>SALVAGE- DEMOLITION OF BUILDINGS</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Total Small Business Set-Aside (FAR 19.5)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>FA442725Q1128</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>HVAC Water Loop Treatment Service - Travis AFB, CA</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Please review the attached Combined Synopsis/Solicitation and attached documents for information on the scope of the service that is required, how to respond to this solicitation, and how quotes will be evaluated. 11 Sept 2025 - Amendment 1 to this solicitation has been posted. This amendment extends the response due date, adds a site visit date, and requires an RFI submission deadline.</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Sep 29, 2025 12:00 PM PDT</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Sep 11, 2025</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Sep 11, 2025</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Combined Synopsis/Solicitation</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Brandon Spratt | Phillip Manwaring</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Plumbing, Heating, and Air-Conditioning Contractors</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>MAINT/REPAIR/REBUILD OF EQUIPMENT- REFRIGERATION, AIR CONDITIONING, AND AIR CIRCULATING EQUIPMENT</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
         <is>
           <t>Total Small Business Set-Aside (FAR 19.5)</t>
         </is>

</xml_diff>